<commit_message>
Second change of priors
Changing binge, F5 and F6 based on examination of chains.
</commit_message>
<xml_diff>
--- a/03_estimate_weights/AUDIT_item_intervals.xlsx
+++ b/03_estimate_weights/AUDIT_item_intervals.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,14 +752,14 @@
         <v>1.5</v>
       </c>
       <c r="G5">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="H5" t="s">
         <v>59</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="2"/>
-        <v>F4 ~ uniform(1.5, 3.5);</v>
+        <v>F4 ~ uniform(1.5, 3);</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
@@ -811,14 +811,14 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="2"/>
-        <v>F5 ~ uniform(3.5, 5.5);</v>
+        <v>F5 ~ uniform(3, 5);</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
@@ -872,14 +872,14 @@
         <v>7</v>
       </c>
       <c r="F7">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>7</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="2"/>
-        <v>F6 ~ uniform(5.5, 7);</v>
+        <v>F6 ~ uniform(5, 7);</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Modifying priors for run 3
</commit_message>
<xml_diff>
--- a/03_estimate_weights/AUDIT_item_intervals.xlsx
+++ b/03_estimate_weights/AUDIT_item_intervals.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
   <si>
     <t>Never</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Y: chains were stuck at minimum (12.5)</t>
+  </si>
+  <si>
+    <t>starting_value3</t>
   </si>
 </sst>
 </file>
@@ -524,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +542,7 @@
     <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -582,8 +585,11 @@
       <c r="O1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -606,7 +612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -656,20 +662,28 @@
         <f t="shared" ref="O3:O13" si="1">(E3-D3)/1.5 +D3</f>
         <v>0.19178082191780821</v>
       </c>
-      <c r="P3" t="str">
+      <c r="P3">
+        <f>E3-((E3-D3)/1.7)</f>
+        <v>0.16244963738920226</v>
+      </c>
+      <c r="Q3" t="str">
         <f>$A3&amp;" = "&amp;ROUND(N3, 3)&amp;", "</f>
         <v xml:space="preserve">F2 = 0.173, </v>
       </c>
-      <c r="Q3" t="str">
+      <c r="R3" t="str">
         <f>$A3&amp;" = "&amp;ROUND(O3, 3)&amp;", "</f>
         <v xml:space="preserve">F2 = 0.192, </v>
       </c>
       <c r="S3" t="str">
+        <f>$A3&amp;" = "&amp;ROUND(P3, 3)&amp;", "</f>
+        <v xml:space="preserve">F2 = 0.162, </v>
+      </c>
+      <c r="T3" t="str">
         <f>"'"&amp;A2&amp;"', "</f>
         <v xml:space="preserve">'F1', </v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -719,20 +733,28 @@
         <f t="shared" si="1"/>
         <v>0.76712328767123283</v>
       </c>
-      <c r="P4" t="str">
-        <f t="shared" ref="P4:P19" si="4">$A4&amp;" = "&amp;ROUND(N4, 3)&amp;", "</f>
+      <c r="P4">
+        <f t="shared" ref="P4:P19" si="4">E4-((E4-D4)/1.7)</f>
+        <v>0.64979854955680905</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" ref="Q4:Q19" si="5">$A4&amp;" = "&amp;ROUND(N4, 3)&amp;", "</f>
         <v xml:space="preserve">F3 = 0.69, </v>
       </c>
-      <c r="Q4" t="str">
-        <f t="shared" ref="Q4:Q19" si="5">$A4&amp;" = "&amp;ROUND(O4, 3)&amp;", "</f>
+      <c r="R4" t="str">
+        <f t="shared" ref="R4:R19" si="6">$A4&amp;" = "&amp;ROUND(O4, 3)&amp;", "</f>
         <v xml:space="preserve">F3 = 0.767, </v>
       </c>
       <c r="S4" t="str">
-        <f t="shared" ref="S4:S19" si="6">"'"&amp;A3&amp;"', "</f>
+        <f t="shared" ref="S4:S19" si="7">$A4&amp;" = "&amp;ROUND(P4, 3)&amp;", "</f>
+        <v xml:space="preserve">F3 = 0.65, </v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" ref="T4:T19" si="8">"'"&amp;A3&amp;"', "</f>
         <v xml:space="preserve">'F2', </v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -781,20 +803,28 @@
       <c r="O5">
         <v>2.5</v>
       </c>
-      <c r="P5" t="str">
+      <c r="P5">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">F4 = 2.1, </v>
+        <v>2.4117647058823528</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">F4 = 2.1, </v>
+      </c>
+      <c r="R5" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">F4 = 2.5, </v>
       </c>
       <c r="S5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">F4 = 2.412, </v>
+      </c>
+      <c r="T5" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'F3', </v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -842,20 +872,28 @@
         <f t="shared" si="1"/>
         <v>4.666666666666667</v>
       </c>
-      <c r="P6" t="str">
+      <c r="P6">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">F5 = 4.5, </v>
+        <v>4.4117647058823533</v>
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">F5 = 4.5, </v>
+      </c>
+      <c r="R6" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">F5 = 4.667, </v>
       </c>
       <c r="S6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">F5 = 4.412, </v>
+      </c>
+      <c r="T6" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'F4', </v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -896,27 +934,35 @@
         <v>53</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N7:N13" si="7">(E7-D7)/2 +D7</f>
+        <f t="shared" ref="N7:N13" si="9">(E7-D7)/2 +D7</f>
         <v>6.5</v>
       </c>
       <c r="O7">
         <f t="shared" si="1"/>
         <v>6.666666666666667</v>
       </c>
-      <c r="P7" t="str">
+      <c r="P7">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">F6 = 6.5, </v>
+        <v>6.4117647058823533</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">F6 = 6.5, </v>
+      </c>
+      <c r="R7" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">F6 = 6.667, </v>
       </c>
       <c r="S7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">F6 = 6.412, </v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'F5', </v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -936,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G10" si="8">E8+0.5</f>
+        <f t="shared" ref="G8:G10" si="10">E8+0.5</f>
         <v>2.5</v>
       </c>
       <c r="I8" t="str">
@@ -958,27 +1004,35 @@
         <v>54</v>
       </c>
       <c r="N8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.5</v>
       </c>
       <c r="O8">
         <f t="shared" si="1"/>
         <v>1.6666666666666665</v>
       </c>
-      <c r="P8" t="str">
+      <c r="P8">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">Q1 = 1.5, </v>
+        <v>1.4117647058823528</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">Q1 = 1.5, </v>
+      </c>
+      <c r="R8" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">Q1 = 1.667, </v>
       </c>
       <c r="S8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">Q1 = 1.412, </v>
+      </c>
+      <c r="T8" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'F6', </v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -995,11 +1049,11 @@
         <v>4</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:F10" si="9">D9-0.5</f>
+        <f t="shared" ref="F9:F10" si="11">D9-0.5</f>
         <v>2.5</v>
       </c>
       <c r="G9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.5</v>
       </c>
       <c r="I9" t="str">
@@ -1021,27 +1075,35 @@
         <v>49</v>
       </c>
       <c r="N9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.5</v>
       </c>
       <c r="O9">
         <f t="shared" si="1"/>
         <v>3.6666666666666665</v>
       </c>
-      <c r="P9" t="str">
+      <c r="P9">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">Q2 = 3.5, </v>
+        <v>3.4117647058823528</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">Q2 = 3.5, </v>
+      </c>
+      <c r="R9" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">Q2 = 3.667, </v>
       </c>
       <c r="S9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">Q2 = 3.412, </v>
+      </c>
+      <c r="T9" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'Q1', </v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1058,11 +1120,11 @@
         <v>6</v>
       </c>
       <c r="F10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4.5</v>
       </c>
       <c r="G10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.5</v>
       </c>
       <c r="I10" t="str">
@@ -1084,27 +1146,35 @@
         <v>50</v>
       </c>
       <c r="N10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5.5</v>
       </c>
       <c r="O10">
         <f t="shared" si="1"/>
         <v>5.666666666666667</v>
       </c>
-      <c r="P10" t="str">
+      <c r="P10">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">Q3 = 5.5, </v>
+        <v>5.4117647058823533</v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">Q3 = 5.5, </v>
+      </c>
+      <c r="R10" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">Q3 = 5.667, </v>
       </c>
       <c r="S10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">Q3 = 5.412, </v>
+      </c>
+      <c r="T10" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'Q2', </v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1147,27 +1217,35 @@
         <v>51</v>
       </c>
       <c r="N11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="O11">
         <f t="shared" si="1"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="P11" t="str">
+      <c r="P11">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">Q4 = 8, </v>
+        <v>7.8235294117647056</v>
       </c>
       <c r="Q11" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">Q4 = 8, </v>
+      </c>
+      <c r="R11" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">Q4 = 8.333, </v>
       </c>
       <c r="S11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">Q4 = 7.824, </v>
+      </c>
+      <c r="T11" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'Q3', </v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1184,15 +1262,15 @@
         <v>12</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F14" si="10">D12-0.5</f>
+        <f t="shared" ref="F12:F14" si="12">D12-0.5</f>
         <v>9.5</v>
       </c>
       <c r="G12">
-        <v>12</v>
+        <v>11.5</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="2"/>
-        <v>Q5 ~ uniform(9.5, 12);</v>
+        <v>Q5 ~ uniform(9.5, 11.5);</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
@@ -1209,27 +1287,35 @@
         <v>52</v>
       </c>
       <c r="N12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="O12">
         <f t="shared" si="1"/>
         <v>11.333333333333334</v>
       </c>
-      <c r="P12" t="str">
+      <c r="P12">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">Q5 = 11, </v>
+        <v>10.823529411764707</v>
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">Q5 = 11, </v>
+      </c>
+      <c r="R12" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">Q5 = 11.333, </v>
       </c>
       <c r="S12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">Q5 = 10.824, </v>
+      </c>
+      <c r="T12" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'Q4', </v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1246,10 +1332,10 @@
         <v>15</v>
       </c>
       <c r="F13">
-        <v>12</v>
+        <v>11.5</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13" si="11">E13+0.5</f>
+        <f t="shared" ref="G13" si="13">E13+0.5</f>
         <v>15.5</v>
       </c>
       <c r="H13" t="s">
@@ -1257,7 +1343,7 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" si="2"/>
-        <v>Q6 ~ uniform(12, 15.5);</v>
+        <v>Q6 ~ uniform(11.5, 15.5);</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
@@ -1274,27 +1360,35 @@
         <v>53</v>
       </c>
       <c r="N13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="O13">
         <f t="shared" si="1"/>
         <v>14.333333333333334</v>
       </c>
-      <c r="P13" t="str">
+      <c r="P13">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">Q6 = 14, </v>
+        <v>13.823529411764707</v>
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">Q6 = 14, </v>
+      </c>
+      <c r="R13" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">Q6 = 14.333, </v>
       </c>
       <c r="S13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">Q6 = 13.824, </v>
+      </c>
+      <c r="T13" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'Q5', </v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1311,7 +1405,7 @@
         <v>6</v>
       </c>
       <c r="F14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>15.5</v>
       </c>
       <c r="G14">
@@ -1341,20 +1435,27 @@
       <c r="O14">
         <v>21</v>
       </c>
-      <c r="P14" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">Q7 = 20, </v>
+      <c r="P14">
+        <v>19</v>
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">Q7 = 20, </v>
+      </c>
+      <c r="R14" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">Q7 = 21, </v>
       </c>
       <c r="S14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">Q7 = 19, </v>
+      </c>
+      <c r="T14" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'Q6', </v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1400,20 +1501,27 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">V1 = 0, </v>
+      <c r="P15">
+        <v>0.5</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">V1 = 0, </v>
       </c>
+      <c r="R15" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">V1 = 0, </v>
+      </c>
       <c r="S15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">V1 = 0.5, </v>
+      </c>
+      <c r="T15" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'Q7', </v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1460,20 +1568,27 @@
       <c r="O16">
         <v>0.4</v>
       </c>
-      <c r="P16" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">V2 = 0.3, </v>
+      <c r="P16">
+        <v>0.25</v>
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">V2 = 0.3, </v>
+      </c>
+      <c r="R16" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">V2 = 0.4, </v>
       </c>
       <c r="S16" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">V2 = 0.25, </v>
+      </c>
+      <c r="T16" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'V1', </v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1520,20 +1635,27 @@
       <c r="O17">
         <v>0.8</v>
       </c>
-      <c r="P17" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">V3 = 0.7, </v>
+      <c r="P17">
+        <v>0.75</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">V3 = 0.7, </v>
+      </c>
+      <c r="R17" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">V3 = 0.8, </v>
       </c>
       <c r="S17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">V3 = 0.75, </v>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'V2', </v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1579,20 +1701,27 @@
       <c r="O18">
         <v>2.5</v>
       </c>
-      <c r="P18" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">V4 = 2, </v>
+      <c r="P18">
+        <v>1.9</v>
       </c>
       <c r="Q18" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">V4 = 2, </v>
+      </c>
+      <c r="R18" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">V4 = 2.5, </v>
       </c>
       <c r="S18" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">V4 = 1.9, </v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'V3', </v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1639,30 +1768,41 @@
       <c r="O19">
         <v>6</v>
       </c>
-      <c r="P19" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">V5 = 5, </v>
+      <c r="P19">
+        <v>5.5</v>
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">V5 = 5, </v>
+      </c>
+      <c r="R19" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">V5 = 6, </v>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">V5 = 5.5, </v>
+      </c>
+      <c r="T19" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">'V4', </v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="P22" t="str">
-        <f>CONCATENATE("sigma = 10, binge = 6, ", P3,P4, P5, P6, P7, P8, P9, P10, P11, P12, P13, P14, P15, P16, P17, P18, P19)</f>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Q22" t="str">
+        <f>CONCATENATE("sigma = 10, binge = 6, ", Q3,Q4, Q5, Q6, Q7, Q8, Q9, Q10, Q11, Q12, Q13, Q14, Q15, Q16, Q17, Q18, Q19)</f>
         <v xml:space="preserve">sigma = 10, binge = 6, F2 = 0.173, F3 = 0.69, F4 = 2.1, F5 = 4.5, F6 = 6.5, Q1 = 1.5, Q2 = 3.5, Q3 = 5.5, Q4 = 8, Q5 = 11, Q6 = 14, Q7 = 20, V1 = 0, V2 = 0.3, V3 = 0.7, V4 = 2, V5 = 5, </v>
       </c>
-      <c r="Q22" t="str">
-        <f>CONCATENATE("sigma = 12, binge = 8, ", Q3,Q4, Q5, Q6, Q7, Q8, Q9, Q10, Q11, Q12, Q13, Q14, Q15, Q16, Q17, Q18, Q19)</f>
-        <v xml:space="preserve">sigma = 12, binge = 8, F2 = 0.192, F3 = 0.767, F4 = 2.5, F5 = 4.667, F6 = 6.667, Q1 = 1.667, Q2 = 3.667, Q3 = 5.667, Q4 = 8.333, Q5 = 11.333, Q6 = 14.333, Q7 = 21, V1 = 0, V2 = 0.4, V3 = 0.8, V4 = 2.5, V5 = 6, </v>
+      <c r="R22" t="str">
+        <f>CONCATENATE("sigma = 12, binge = 5, ", R3,R4, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19)</f>
+        <v xml:space="preserve">sigma = 12, binge = 5, F2 = 0.192, F3 = 0.767, F4 = 2.5, F5 = 4.667, F6 = 6.667, Q1 = 1.667, Q2 = 3.667, Q3 = 5.667, Q4 = 8.333, Q5 = 11.333, Q6 = 14.333, Q7 = 21, V1 = 0, V2 = 0.4, V3 = 0.8, V4 = 2.5, V5 = 6, </v>
       </c>
       <c r="S22" t="str">
-        <f>CONCATENATE(S3,S4, S5, S6, S7, S8, S9, S10, S11, S12, S13, S14, S15, S16, S17, S18, S19)</f>
+        <f>CONCATENATE("sigma = 8, binge = 7, ", S3,S4, S5, S6, S7, S8, S9, S10, S11, S12, S13, S14, S15, S16, S17, S18, S19)</f>
+        <v xml:space="preserve">sigma = 8, binge = 7, F2 = 0.162, F3 = 0.65, F4 = 2.412, F5 = 4.412, F6 = 6.412, Q1 = 1.412, Q2 = 3.412, Q3 = 5.412, Q4 = 7.824, Q5 = 10.824, Q6 = 13.824, Q7 = 19, V1 = 0.5, V2 = 0.25, V3 = 0.75, V4 = 1.9, V5 = 5.5, </v>
+      </c>
+      <c r="T22" t="str">
+        <f>CONCATENATE(T3,T4, T5, T6, T7, T8, T9, T10, T11, T12, T13, T14, T15, T16, T17, T18, T19)</f>
         <v xml:space="preserve">'F1', 'F2', 'F3', 'F4', 'F5', 'F6', 'Q1', 'Q2', 'Q3', 'Q4', 'Q5', 'Q6', 'Q7', 'V1', 'V2', 'V3', 'V4', </v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix out-of-bound chain init value (run 3)
</commit_message>
<xml_diff>
--- a/03_estimate_weights/AUDIT_item_intervals.xlsx
+++ b/03_estimate_weights/AUDIT_item_intervals.xlsx
@@ -530,7 +530,7 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,6 +540,7 @@
     <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -734,7 +735,7 @@
         <v>0.76712328767123283</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P19" si="4">E4-((E4-D4)/1.7)</f>
+        <f t="shared" ref="P4:P13" si="4">E4-((E4-D4)/1.7)</f>
         <v>0.64979854955680905</v>
       </c>
       <c r="Q4" t="str">
@@ -1502,7 +1503,7 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="5"/>
@@ -1514,7 +1515,7 @@
       </c>
       <c r="S15" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">V1 = 0.5, </v>
+        <v xml:space="preserve">V1 = 0.05, </v>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="8"/>
@@ -1799,7 +1800,7 @@
       </c>
       <c r="S22" t="str">
         <f>CONCATENATE("sigma = 8, binge = 7, ", S3,S4, S5, S6, S7, S8, S9, S10, S11, S12, S13, S14, S15, S16, S17, S18, S19)</f>
-        <v xml:space="preserve">sigma = 8, binge = 7, F2 = 0.162, F3 = 0.65, F4 = 2.412, F5 = 4.412, F6 = 6.412, Q1 = 1.412, Q2 = 3.412, Q3 = 5.412, Q4 = 7.824, Q5 = 10.824, Q6 = 13.824, Q7 = 19, V1 = 0.5, V2 = 0.25, V3 = 0.75, V4 = 1.9, V5 = 5.5, </v>
+        <v xml:space="preserve">sigma = 8, binge = 7, F2 = 0.162, F3 = 0.65, F4 = 2.412, F5 = 4.412, F6 = 6.412, Q1 = 1.412, Q2 = 3.412, Q3 = 5.412, Q4 = 7.824, Q5 = 10.824, Q6 = 13.824, Q7 = 19, V1 = 0.05, V2 = 0.25, V3 = 0.75, V4 = 1.9, V5 = 5.5, </v>
       </c>
       <c r="T22" t="str">
         <f>CONCATENATE(T3,T4, T5, T6, T7, T8, T9, T10, T11, T12, T13, T14, T15, T16, T17, T18, T19)</f>

</xml_diff>

<commit_message>
preparing for fifth run
raised upper bound for Q3 from 6.5 to 7
lowered lower bound for Q6 further from 10 down to 9.5.
</commit_message>
<xml_diff>
--- a/03_estimate_weights/AUDIT_item_intervals.xlsx
+++ b/03_estimate_weights/AUDIT_item_intervals.xlsx
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W26" sqref="W26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,12 +1327,11 @@
         <v>4.5</v>
       </c>
       <c r="G10">
-        <f t="shared" si="17"/>
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="4"/>
-        <v>Q3 ~ uniform(4.5, 6.5);</v>
+        <v>Q3 ~ uniform(4.5, 7);</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -1382,19 +1381,19 @@
       </c>
       <c r="U10" t="str">
         <f t="shared" si="10"/>
-        <v>real Q3 =  ((Q3hyper * 2) + 4.5);</v>
+        <v>real Q3 =  ((Q3hyper * 2.5) + 4.5);</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">Q3hyper = 0.5, </v>
+        <v xml:space="preserve">Q3hyper = 0.4, </v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">Q3hyper = 0.583, </v>
+        <v xml:space="preserve">Q3hyper = 0.467, </v>
       </c>
       <c r="X10" t="str">
         <f t="shared" si="13"/>
-        <v xml:space="preserve">Q3hyper = 0.456, </v>
+        <v xml:space="preserve">Q3hyper = 0.365, </v>
       </c>
       <c r="Y10" t="str">
         <f t="shared" si="14"/>
@@ -1607,7 +1606,7 @@
         <v>15</v>
       </c>
       <c r="F13">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="G13">
         <f t="shared" ref="G13" si="20">E13+0.5</f>
@@ -1615,7 +1614,7 @@
       </c>
       <c r="H13" t="str">
         <f t="shared" si="4"/>
-        <v>Q6 ~ uniform(10, 15.5);</v>
+        <v>Q6 ~ uniform(9.5, 15.5);</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
@@ -1665,19 +1664,19 @@
       </c>
       <c r="U13" t="str">
         <f t="shared" si="10"/>
-        <v>real Q6 =  ((Q6hyper * 5.5) + 10);</v>
+        <v>real Q6 =  ((Q6hyper * 6) + 9.5);</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">Q6hyper = 0.727, </v>
+        <v xml:space="preserve">Q6hyper = 0.75, </v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">Q6hyper = 0.788, </v>
+        <v xml:space="preserve">Q6hyper = 0.806, </v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="13"/>
-        <v xml:space="preserve">Q6hyper = 0.695, </v>
+        <v xml:space="preserve">Q6hyper = 0.721, </v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="14"/>
@@ -2247,15 +2246,15 @@
       </c>
       <c r="V22" t="str">
         <f>CONCATENATE("sigma = 10, binge = 6, ", V3,V4, V5, V6, V7, V8, V9, V10, V11, V12, V13, V14, V15, V16, V17, V18, V19)</f>
-        <v xml:space="preserve">sigma = 10, binge = 6, F2hyper = 0.182, F3hyper = 0.19, F4hyper = 0.4, F5hyper = 0.75, F6hyper = 0.75, Q1hyper = 0.333, Q2hyper = 0.5, Q3hyper = 0.5, Q4hyper = 0.5, Q5hyper = 0.75, Q6hyper = 0.727, Q7hyper = 0.474, V1hyper = 0.01, V2hyper = 0.5, V3hyper = 0.4, V4hyper = 0.5, V5hyper = 0.5, </v>
+        <v xml:space="preserve">sigma = 10, binge = 6, F2hyper = 0.182, F3hyper = 0.19, F4hyper = 0.4, F5hyper = 0.75, F6hyper = 0.75, Q1hyper = 0.333, Q2hyper = 0.5, Q3hyper = 0.4, Q4hyper = 0.5, Q5hyper = 0.75, Q6hyper = 0.75, Q7hyper = 0.474, V1hyper = 0.01, V2hyper = 0.5, V3hyper = 0.4, V4hyper = 0.5, V5hyper = 0.5, </v>
       </c>
       <c r="W22" t="str">
         <f>CONCATENATE("sigma = 12, binge = 5, ", W3,W4, W5, W6, W7, W8, W9, W10, W11, W12, W13, W14, W15, W16, W17, W18, W19)</f>
-        <v xml:space="preserve">sigma = 12, binge = 5, F2hyper = 0.229, F3hyper = 0.267, F4hyper = 0.667, F5hyper = 0.833, F6hyper = 0.833, Q1hyper = 0.444, Q2hyper = 0.583, Q3hyper = 0.583, Q4hyper = 0.611, Q5hyper = 0.917, Q6hyper = 0.788, Q7hyper = 0.579, V1hyper = 0.1, V2hyper = 0.75, V3hyper = 0.6, V4hyper = 0.75, V5hyper = 0.75, </v>
+        <v xml:space="preserve">sigma = 12, binge = 5, F2hyper = 0.229, F3hyper = 0.267, F4hyper = 0.667, F5hyper = 0.833, F6hyper = 0.833, Q1hyper = 0.444, Q2hyper = 0.583, Q3hyper = 0.467, Q4hyper = 0.611, Q5hyper = 0.917, Q6hyper = 0.806, Q7hyper = 0.579, V1hyper = 0.1, V2hyper = 0.75, V3hyper = 0.6, V4hyper = 0.75, V5hyper = 0.75, </v>
       </c>
       <c r="X22" t="str">
         <f>CONCATENATE("sigma = 8, binge = 7, ", X3,X4, X5, X6, X7, X8, X9, X10, X11, X12, X13, X14, X15, X16, X17, X18, X19)</f>
-        <v xml:space="preserve">sigma = 8, binge = 7, F2hyper = 0.156, F3hyper = 0.15, F4hyper = 0.608, F5hyper = 0.706, F6hyper = 0.706, Q1hyper = 0.275, Q2hyper = 0.456, Q3hyper = 0.456, Q4hyper = 0.441, Q5hyper = 0.662, Q6hyper = 0.695, Q7hyper = 0.368, V1hyper = 0.5, V2hyper = 0.375, V3hyper = 0.5, V4hyper = 0.45, V5hyper = 0.625, </v>
+        <v xml:space="preserve">sigma = 8, binge = 7, F2hyper = 0.156, F3hyper = 0.15, F4hyper = 0.608, F5hyper = 0.706, F6hyper = 0.706, Q1hyper = 0.275, Q2hyper = 0.456, Q3hyper = 0.365, Q4hyper = 0.441, Q5hyper = 0.662, Q6hyper = 0.721, Q7hyper = 0.368, V1hyper = 0.5, V2hyper = 0.375, V3hyper = 0.5, V4hyper = 0.45, V5hyper = 0.625, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sixth run: fixed the prior on binge drinking
</commit_message>
<xml_diff>
--- a/03_estimate_weights/AUDIT_item_intervals.xlsx
+++ b/03_estimate_weights/AUDIT_item_intervals.xlsx
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G10" si="17">E8+0.5</f>
+        <f t="shared" ref="G8:G9" si="17">E8+0.5</f>
         <v>2.5</v>
       </c>
       <c r="H8" t="str">
@@ -2245,16 +2245,16 @@
         <v xml:space="preserve">'F1', 'F2', 'F3', 'F4', 'F5', 'F6', 'Q1', 'Q2', 'Q3', 'Q4', 'Q5', 'Q6', 'Q7', 'V1', 'V2', 'V3', 'V4', </v>
       </c>
       <c r="V22" t="str">
-        <f>CONCATENATE("sigma = 10, binge = 6, ", V3,V4, V5, V6, V7, V8, V9, V10, V11, V12, V13, V14, V15, V16, V17, V18, V19)</f>
-        <v xml:space="preserve">sigma = 10, binge = 6, F2hyper = 0.182, F3hyper = 0.19, F4hyper = 0.4, F5hyper = 0.75, F6hyper = 0.75, Q1hyper = 0.333, Q2hyper = 0.5, Q3hyper = 0.4, Q4hyper = 0.5, Q5hyper = 0.75, Q6hyper = 0.75, Q7hyper = 0.474, V1hyper = 0.01, V2hyper = 0.5, V3hyper = 0.4, V4hyper = 0.5, V5hyper = 0.5, </v>
+        <f>CONCATENATE("sigma = 10, bingehyper = 1, ", V3,V4, V5, V6, V7, V8, V9, V10, V11, V12, V13, V14, V15, V16, V17, V18, V19)</f>
+        <v xml:space="preserve">sigma = 10, bingehyper = 1, F2hyper = 0.182, F3hyper = 0.19, F4hyper = 0.4, F5hyper = 0.75, F6hyper = 0.75, Q1hyper = 0.333, Q2hyper = 0.5, Q3hyper = 0.4, Q4hyper = 0.5, Q5hyper = 0.75, Q6hyper = 0.75, Q7hyper = 0.474, V1hyper = 0.01, V2hyper = 0.5, V3hyper = 0.4, V4hyper = 0.5, V5hyper = 0.5, </v>
       </c>
       <c r="W22" t="str">
-        <f>CONCATENATE("sigma = 12, binge = 5, ", W3,W4, W5, W6, W7, W8, W9, W10, W11, W12, W13, W14, W15, W16, W17, W18, W19)</f>
-        <v xml:space="preserve">sigma = 12, binge = 5, F2hyper = 0.229, F3hyper = 0.267, F4hyper = 0.667, F5hyper = 0.833, F6hyper = 0.833, Q1hyper = 0.444, Q2hyper = 0.583, Q3hyper = 0.467, Q4hyper = 0.611, Q5hyper = 0.917, Q6hyper = 0.806, Q7hyper = 0.579, V1hyper = 0.1, V2hyper = 0.75, V3hyper = 0.6, V4hyper = 0.75, V5hyper = 0.75, </v>
+        <f>CONCATENATE("sigma = 12, bingehyper = 0, ", W3,W4, W5, W6, W7, W8, W9, W10, W11, W12, W13, W14, W15, W16, W17, W18, W19)</f>
+        <v xml:space="preserve">sigma = 12, bingehyper = 0, F2hyper = 0.229, F3hyper = 0.267, F4hyper = 0.667, F5hyper = 0.833, F6hyper = 0.833, Q1hyper = 0.444, Q2hyper = 0.583, Q3hyper = 0.467, Q4hyper = 0.611, Q5hyper = 0.917, Q6hyper = 0.806, Q7hyper = 0.579, V1hyper = 0.1, V2hyper = 0.75, V3hyper = 0.6, V4hyper = 0.75, V5hyper = 0.75, </v>
       </c>
       <c r="X22" t="str">
-        <f>CONCATENATE("sigma = 8, binge = 7, ", X3,X4, X5, X6, X7, X8, X9, X10, X11, X12, X13, X14, X15, X16, X17, X18, X19)</f>
-        <v xml:space="preserve">sigma = 8, binge = 7, F2hyper = 0.156, F3hyper = 0.15, F4hyper = 0.608, F5hyper = 0.706, F6hyper = 0.706, Q1hyper = 0.275, Q2hyper = 0.456, Q3hyper = 0.365, Q4hyper = 0.441, Q5hyper = 0.662, Q6hyper = 0.721, Q7hyper = 0.368, V1hyper = 0.5, V2hyper = 0.375, V3hyper = 0.5, V4hyper = 0.45, V5hyper = 0.625, </v>
+        <f>CONCATENATE("sigma = 8, bingehyper = 2, ", X3,X4, X5, X6, X7, X8, X9, X10, X11, X12, X13, X14, X15, X16, X17, X18, X19)</f>
+        <v xml:space="preserve">sigma = 8, bingehyper = 2, F2hyper = 0.156, F3hyper = 0.15, F4hyper = 0.608, F5hyper = 0.706, F6hyper = 0.706, Q1hyper = 0.275, Q2hyper = 0.456, Q3hyper = 0.365, Q4hyper = 0.441, Q5hyper = 0.662, Q6hyper = 0.721, Q7hyper = 0.368, V1hyper = 0.5, V2hyper = 0.375, V3hyper = 0.5, V4hyper = 0.45, V5hyper = 0.625, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
preparing eighth run: simple QFV
return Q3 to nominal interval
adjust V1 which maxed out in initial test
</commit_message>
<xml_diff>
--- a/03_estimate_weights/AUDIT_item_intervals.xlsx
+++ b/03_estimate_weights/AUDIT_item_intervals.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="9165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="8700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y22" sqref="Y22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,11 +1327,11 @@
         <v>4.5</v>
       </c>
       <c r="G10">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="4"/>
-        <v>Q3 ~ uniform(4.5, 6);</v>
+        <v>Q3 ~ uniform(4.5, 6.5);</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -1381,19 +1381,19 @@
       </c>
       <c r="U10" t="str">
         <f t="shared" si="10"/>
-        <v>real Q3 =  ((Q3hyper * 1.5) + 4.5);</v>
+        <v>real Q3 =  ((Q3hyper * 2) + 4.5);</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">Q3hyper = 0.667, </v>
+        <v xml:space="preserve">Q3hyper = 0.5, </v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">Q3hyper = 0.778, </v>
+        <v xml:space="preserve">Q3hyper = 0.583, </v>
       </c>
       <c r="X10" t="str">
         <f t="shared" si="13"/>
-        <v xml:space="preserve">Q3hyper = 0.608, </v>
+        <v xml:space="preserve">Q3hyper = 0.456, </v>
       </c>
       <c r="Y10" t="str">
         <f t="shared" si="14"/>
@@ -1793,11 +1793,11 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="4"/>
-        <v>V1 ~ uniform(0, 0.1);</v>
+        <v>V1 ~ uniform(0, 0.2);</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
@@ -1844,19 +1844,19 @@
       </c>
       <c r="U15" t="str">
         <f t="shared" si="10"/>
-        <v>real V1 =  ((V1hyper * 0.1) + 0);</v>
+        <v>real V1 =  ((V1hyper * 0.2) + 0);</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">V1hyper = 0.01, </v>
+        <v xml:space="preserve">V1hyper = 0.005, </v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">V1hyper = 0.1, </v>
+        <v xml:space="preserve">V1hyper = 0.05, </v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="13"/>
-        <v xml:space="preserve">V1hyper = 0.5, </v>
+        <v xml:space="preserve">V1hyper = 0.25, </v>
       </c>
       <c r="Y15" t="str">
         <f t="shared" si="14"/>
@@ -1881,14 +1881,14 @@
         <v>0.11506849315068493</v>
       </c>
       <c r="F16">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G16">
         <v>0.5</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="4"/>
-        <v>V2 ~ uniform(0.1, 0.5);</v>
+        <v>V2 ~ uniform(0.2, 0.5);</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
@@ -1935,19 +1935,19 @@
       </c>
       <c r="U16" t="str">
         <f t="shared" si="10"/>
-        <v>real V2 =  ((V2hyper * 0.4) + 0.1);</v>
+        <v>real V2 =  ((V2hyper * 0.3) + 0.2);</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">V2hyper = 0.5, </v>
+        <v xml:space="preserve">V2hyper = 0.333, </v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">V2hyper = 0.75, </v>
+        <v xml:space="preserve">V2hyper = 0.667, </v>
       </c>
       <c r="X16" t="str">
         <f t="shared" si="13"/>
-        <v xml:space="preserve">V2hyper = 0.375, </v>
+        <v xml:space="preserve">V2hyper = 0.167, </v>
       </c>
       <c r="Y16" t="str">
         <f t="shared" si="14"/>
@@ -2245,15 +2245,15 @@
       </c>
       <c r="V22" t="str">
         <f>CONCATENATE("sigma = 10, bingehyper = 1, ", V3,V4, V5, V6, V7, V8, V9, V10, V11, V12, V13, V14, V15, V16, V17, V18, V19)</f>
-        <v xml:space="preserve">sigma = 10, bingehyper = 1, F2hyper = 0.182, F3hyper = 0.19, F4hyper = 0.4, F5hyper = 0.75, F6hyper = 0.75, Q1hyper = 0.333, Q2hyper = 0.5, Q3hyper = 0.667, Q4hyper = 0.5, Q5hyper = 0.75, Q6hyper = 0.75, Q7hyper = 0.474, V1hyper = 0.01, V2hyper = 0.5, V3hyper = 0.4, V4hyper = 0.5, V5hyper = 0.5, </v>
+        <v xml:space="preserve">sigma = 10, bingehyper = 1, F2hyper = 0.182, F3hyper = 0.19, F4hyper = 0.4, F5hyper = 0.75, F6hyper = 0.75, Q1hyper = 0.333, Q2hyper = 0.5, Q3hyper = 0.5, Q4hyper = 0.5, Q5hyper = 0.75, Q6hyper = 0.75, Q7hyper = 0.474, V1hyper = 0.005, V2hyper = 0.333, V3hyper = 0.4, V4hyper = 0.5, V5hyper = 0.5, </v>
       </c>
       <c r="W22" t="str">
         <f>CONCATENATE("sigma = 12, bingehyper = 0, ", W3,W4, W5, W6, W7, W8, W9, W10, W11, W12, W13, W14, W15, W16, W17, W18, W19)</f>
-        <v xml:space="preserve">sigma = 12, bingehyper = 0, F2hyper = 0.229, F3hyper = 0.267, F4hyper = 0.667, F5hyper = 0.833, F6hyper = 0.833, Q1hyper = 0.444, Q2hyper = 0.583, Q3hyper = 0.778, Q4hyper = 0.611, Q5hyper = 0.917, Q6hyper = 0.806, Q7hyper = 0.579, V1hyper = 0.1, V2hyper = 0.75, V3hyper = 0.6, V4hyper = 0.75, V5hyper = 0.75, </v>
+        <v xml:space="preserve">sigma = 12, bingehyper = 0, F2hyper = 0.229, F3hyper = 0.267, F4hyper = 0.667, F5hyper = 0.833, F6hyper = 0.833, Q1hyper = 0.444, Q2hyper = 0.583, Q3hyper = 0.583, Q4hyper = 0.611, Q5hyper = 0.917, Q6hyper = 0.806, Q7hyper = 0.579, V1hyper = 0.05, V2hyper = 0.667, V3hyper = 0.6, V4hyper = 0.75, V5hyper = 0.75, </v>
       </c>
       <c r="X22" t="str">
         <f>CONCATENATE("sigma = 8, bingehyper = 2, ", X3,X4, X5, X6, X7, X8, X9, X10, X11, X12, X13, X14, X15, X16, X17, X18, X19)</f>
-        <v xml:space="preserve">sigma = 8, bingehyper = 2, F2hyper = 0.156, F3hyper = 0.15, F4hyper = 0.608, F5hyper = 0.706, F6hyper = 0.706, Q1hyper = 0.275, Q2hyper = 0.456, Q3hyper = 0.608, Q4hyper = 0.441, Q5hyper = 0.662, Q6hyper = 0.721, Q7hyper = 0.368, V1hyper = 0.5, V2hyper = 0.375, V3hyper = 0.5, V4hyper = 0.45, V5hyper = 0.625, </v>
+        <v xml:space="preserve">sigma = 8, bingehyper = 2, F2hyper = 0.156, F3hyper = 0.15, F4hyper = 0.608, F5hyper = 0.706, F6hyper = 0.706, Q1hyper = 0.275, Q2hyper = 0.456, Q3hyper = 0.456, Q4hyper = 0.441, Q5hyper = 0.662, Q6hyper = 0.721, Q7hyper = 0.368, V1hyper = 0.25, V2hyper = 0.167, V3hyper = 0.5, V4hyper = 0.45, V5hyper = 0.625, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>